<commit_message>
Updated project_system with changes
</commit_message>
<xml_diff>
--- a/projects.xlsx
+++ b/projects.xlsx
@@ -595,60 +595,54 @@
           <t>2025-02-28</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>صح</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>2025-02-25</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>صح</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>عطاء22222</t>
-        </is>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>صح</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>2025-02-27</t>
-        </is>
+          <t>2025-02-28</t>
+        </is>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>صح</t>
+          <t>✅</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>صح</t>
+          <t>✅</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>صح</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr"/>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>صح</t>
+          <t>✅</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>صح</t>
+          <t>✅</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">

</xml_diff>